<commit_message>
update to weekly report
</commit_message>
<xml_diff>
--- a/Weekly Reports/Strategy Team Report.xlsx
+++ b/Weekly Reports/Strategy Team Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="105">
   <si>
     <t>PHASE ONE</t>
   </si>
@@ -343,7 +343,7 @@
     <t>Gabe/Isaiah</t>
   </si>
   <si>
-    <t xml:space="preserve">This week we accomplised the entirety of the basic control system for the mavric rover simulator. As well as  discussing the ideas of an ir camera for the science team's spectrometer. (anti mass) We have also started outlining the website changes we will be making as soon as I have access to the mavric page. Which includes, changing the photos to reflect the current team, and editing the team pages. </t>
+    <t>Isaiah has done major overhaul to the M2I mavric website. The basic controls progress has been moved slightly off due to needing to rewrite the new controller to make it worth with tank drive. We have been discussing with the other teams about the change of MAVRIC's battery and motors, which will  be finalized tomorrow 10/14. Details of which will be added to the next weekly report even though a bulk of the discussion was done this week (in order to be sure of the final outcome)</t>
   </si>
 </sst>
 </file>
@@ -431,29 +431,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -505,6 +482,29 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1109,31 +1109,100 @@
     <xf numFmtId="0" fontId="4" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="19" fillId="24" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="19" fillId="24" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1161,15 +1230,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1188,12 +1248,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1212,85 +1266,29 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="22" fillId="24" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="22" fillId="24" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1912,174 +1910,174 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="A4" s="86"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="77"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
+      <c r="A10" s="86"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
+      <c r="A11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2096,408 +2094,419 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="111" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="111"/>
+    <col min="1" max="1" width="32.875" style="66" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="66"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="65" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="114" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="112" t="s">
+    <row r="2" spans="1:5" s="67" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A2" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="118"/>
+      <c r="C4" s="90"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="118"/>
+      <c r="C5" s="90"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="118"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="119">
-        <v>7</v>
+      <c r="B7" s="71">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="72" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="122">
+      <c r="B9" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="122">
+      <c r="B10" s="74">
         <f>COUNTIF('Attendance Records'!D2:Q9,"NP")</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="72" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="125" t="s">
+      <c r="A13" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="125"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="135" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="126"/>
-      <c r="B15" s="126"/>
-      <c r="C15" s="126"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="126"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="126"/>
-      <c r="B16" s="126"/>
-      <c r="C16" s="126"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="126"/>
-      <c r="B17" s="126"/>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="126"/>
-      <c r="B18" s="126"/>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="126"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="126"/>
-      <c r="B20" s="126"/>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="127" t="s">
+      <c r="A21" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="128"/>
-      <c r="C21" s="128"/>
-      <c r="D21" s="128"/>
-      <c r="E21" s="128"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="129" t="s">
+      <c r="B22" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="129" t="s">
+      <c r="D22" s="79" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="124" t="str">
+      <c r="A23" s="76" t="str">
         <f>'Team Task Chart'!C5</f>
         <v>MAVRIC Team Technical Advising</v>
       </c>
-      <c r="B23" s="130">
+      <c r="B23" s="80">
         <f>'Team Task Chart'!F5</f>
         <v>43070</v>
       </c>
-      <c r="C23" s="131">
-        <v>0.1</v>
-      </c>
-      <c r="D23" s="124" t="s">
+      <c r="C23" s="81">
+        <f>'Team Task Chart'!H5</f>
+        <v>4.3333333333333335E-2</v>
+      </c>
+      <c r="D23" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="124" t="str">
+      <c r="A24" s="76" t="str">
         <f>'Team Task Chart'!C6</f>
         <v>Advise E-Team</v>
       </c>
-      <c r="B24" s="130">
+      <c r="B24" s="80">
         <f>'Team Task Chart'!F6</f>
         <v>43070</v>
       </c>
-      <c r="C24" s="131">
-        <v>0.04</v>
-      </c>
-      <c r="D24" s="124" t="s">
+      <c r="C24" s="81">
+        <f>'Team Task Chart'!H6</f>
+        <v>0.06</v>
+      </c>
+      <c r="D24" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="124" t="str">
+      <c r="A25" s="76" t="str">
         <f>'Team Task Chart'!C7</f>
         <v>Advise Science Team</v>
       </c>
-      <c r="B25" s="130">
+      <c r="B25" s="80">
         <f>'Team Task Chart'!F7</f>
         <v>43070</v>
       </c>
-      <c r="C25" s="131">
+      <c r="C25" s="81">
+        <f>'Team Task Chart'!H7</f>
         <v>0.02</v>
       </c>
-      <c r="D25" s="124" t="s">
+      <c r="D25" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="124" t="str">
+      <c r="A26" s="76" t="str">
         <f>'Team Task Chart'!C8</f>
         <v>Advise Mechanical Team</v>
       </c>
-      <c r="B26" s="130">
+      <c r="B26" s="80">
         <f>'Team Task Chart'!F8</f>
         <v>43070</v>
       </c>
-      <c r="C26" s="131">
-        <v>0.04</v>
-      </c>
-      <c r="D26" s="124" t="s">
+      <c r="C26" s="81">
+        <f>'Team Task Chart'!H8</f>
+        <v>0.05</v>
+      </c>
+      <c r="D26" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="124" t="str">
+      <c r="A27" s="76" t="str">
         <f>'Team Task Chart'!C13</f>
         <v xml:space="preserve">Rover Simulator </v>
       </c>
-      <c r="B27" s="130">
+      <c r="B27" s="80">
         <f>'Team Task Chart'!F13</f>
         <v>43057</v>
       </c>
-      <c r="C27" s="131">
-        <v>0.1</v>
-      </c>
-      <c r="D27" s="124" t="s">
+      <c r="C27" s="81">
+        <f>'Team Task Chart'!H13</f>
+        <v>0.25</v>
+      </c>
+      <c r="D27" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="124" t="str">
+      <c r="A28" s="76" t="str">
         <f>'Team Task Chart'!C14</f>
         <v>Basic controls</v>
       </c>
-      <c r="B28" s="130">
+      <c r="B28" s="80">
         <f>'Team Task Chart'!F14</f>
         <v>43014</v>
       </c>
-      <c r="C28" s="131">
-        <v>0.05</v>
-      </c>
-      <c r="D28" s="124" t="s">
-        <v>60</v>
+      <c r="C28" s="81">
+        <f>'Team Task Chart'!H14</f>
+        <v>0.95</v>
+      </c>
+      <c r="D28" s="136" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="124" t="str">
+      <c r="A29" s="76" t="str">
         <f>'Team Task Chart'!C15</f>
         <v>Camera feedback</v>
       </c>
-      <c r="B29" s="130">
+      <c r="B29" s="80">
         <f>'Team Task Chart'!F15</f>
         <v>43022</v>
       </c>
-      <c r="C29" s="131">
+      <c r="C29" s="81">
+        <f>'Team Task Chart'!H15</f>
         <v>0</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="124" t="str">
+      <c r="A30" s="76" t="str">
         <f>'Team Task Chart'!C16</f>
         <v>Rover rigging</v>
       </c>
-      <c r="B30" s="130">
+      <c r="B30" s="80">
         <f>'Team Task Chart'!F16</f>
         <v>43036</v>
       </c>
-      <c r="C30" s="131">
+      <c r="C30" s="81">
+        <f>'Team Task Chart'!H16</f>
         <v>0.05</v>
       </c>
-      <c r="D30" s="124" t="s">
+      <c r="D30" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="124" t="str">
+      <c r="A31" s="76" t="str">
         <f>'Team Task Chart'!C18</f>
         <v>MAVRIC Cockpit</v>
       </c>
-      <c r="B31" s="130">
+      <c r="B31" s="80">
         <f>'Team Task Chart'!F18</f>
         <v>43036</v>
       </c>
-      <c r="C31" s="131">
-        <v>0.05</v>
-      </c>
-      <c r="D31" s="124" t="s">
+      <c r="C31" s="81">
+        <f>'Team Task Chart'!H18</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D31" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="124" t="str">
+      <c r="A32" s="76" t="str">
         <f>'Team Task Chart'!C19</f>
         <v>Decide on Cockpit style</v>
       </c>
-      <c r="B32" s="130">
+      <c r="B32" s="80">
         <f>'Team Task Chart'!F19</f>
         <v>43022</v>
       </c>
-      <c r="C32" s="131">
+      <c r="C32" s="81">
+        <f>'Team Task Chart'!H19</f>
         <v>0.05</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="124" t="str">
+      <c r="A33" s="76" t="str">
         <f>'Team Task Chart'!C20</f>
         <v>Build control system/hardware</v>
       </c>
-      <c r="B33" s="130">
+      <c r="B33" s="80">
         <f>'Team Task Chart'!F20</f>
         <v>43036</v>
       </c>
-      <c r="C33" s="131">
+      <c r="C33" s="81">
+        <f>'Team Task Chart'!H20</f>
         <v>0</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="124"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="131"/>
-      <c r="D34" s="124"/>
+      <c r="A34" s="76"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="76"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="132"/>
-      <c r="B35" s="133"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="132"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="82"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="132"/>
-      <c r="B36" s="133"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="132"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="82"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="132"/>
-      <c r="B37" s="133"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="132"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="82"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="124"/>
-      <c r="B38" s="130"/>
-      <c r="C38" s="131"/>
-      <c r="D38" s="124"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="76"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="124"/>
-      <c r="B39" s="130"/>
-      <c r="C39" s="131"/>
-      <c r="D39" s="124"/>
+      <c r="A39" s="76"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="76"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="124"/>
-      <c r="B40" s="130"/>
-      <c r="C40" s="131"/>
-      <c r="D40" s="124"/>
+      <c r="A40" s="76"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2622,7 +2631,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2647,7 +2656,7 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2747,228 +2756,228 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="81" t="s">
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82"/>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82"/>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82"/>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
-      <c r="AL2" s="83"/>
-      <c r="AM2" s="84" t="s">
+      <c r="Y2" s="107"/>
+      <c r="Z2" s="107"/>
+      <c r="AA2" s="107"/>
+      <c r="AB2" s="107"/>
+      <c r="AC2" s="107"/>
+      <c r="AD2" s="107"/>
+      <c r="AE2" s="107"/>
+      <c r="AF2" s="107"/>
+      <c r="AG2" s="107"/>
+      <c r="AH2" s="107"/>
+      <c r="AI2" s="107"/>
+      <c r="AJ2" s="107"/>
+      <c r="AK2" s="107"/>
+      <c r="AL2" s="108"/>
+      <c r="AM2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="85"/>
-      <c r="AS2" s="85"/>
-      <c r="AT2" s="85"/>
-      <c r="AU2" s="85"/>
-      <c r="AV2" s="85"/>
-      <c r="AW2" s="85"/>
-      <c r="AX2" s="85"/>
-      <c r="AY2" s="85"/>
-      <c r="AZ2" s="85"/>
-      <c r="BA2" s="86"/>
-      <c r="BB2" s="87" t="s">
+      <c r="AN2" s="110"/>
+      <c r="AO2" s="110"/>
+      <c r="AP2" s="110"/>
+      <c r="AQ2" s="110"/>
+      <c r="AR2" s="110"/>
+      <c r="AS2" s="110"/>
+      <c r="AT2" s="110"/>
+      <c r="AU2" s="110"/>
+      <c r="AV2" s="110"/>
+      <c r="AW2" s="110"/>
+      <c r="AX2" s="110"/>
+      <c r="AY2" s="110"/>
+      <c r="AZ2" s="110"/>
+      <c r="BA2" s="111"/>
+      <c r="BB2" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="88"/>
-      <c r="BD2" s="88"/>
-      <c r="BE2" s="88"/>
-      <c r="BF2" s="88"/>
-      <c r="BG2" s="88"/>
-      <c r="BH2" s="88"/>
-      <c r="BI2" s="88"/>
-      <c r="BJ2" s="88"/>
-      <c r="BK2" s="88"/>
-      <c r="BL2" s="88"/>
-      <c r="BM2" s="88"/>
-      <c r="BN2" s="88"/>
-      <c r="BO2" s="88"/>
-      <c r="BP2" s="89"/>
-      <c r="BQ2" s="87" t="s">
+      <c r="BC2" s="95"/>
+      <c r="BD2" s="95"/>
+      <c r="BE2" s="95"/>
+      <c r="BF2" s="95"/>
+      <c r="BG2" s="95"/>
+      <c r="BH2" s="95"/>
+      <c r="BI2" s="95"/>
+      <c r="BJ2" s="95"/>
+      <c r="BK2" s="95"/>
+      <c r="BL2" s="95"/>
+      <c r="BM2" s="95"/>
+      <c r="BN2" s="95"/>
+      <c r="BO2" s="95"/>
+      <c r="BP2" s="96"/>
+      <c r="BQ2" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="BR2" s="88"/>
-      <c r="BS2" s="88"/>
-      <c r="BT2" s="88"/>
-      <c r="BU2" s="88"/>
-      <c r="BV2" s="88"/>
-      <c r="BW2" s="88"/>
-      <c r="BX2" s="88"/>
-      <c r="BY2" s="88"/>
-      <c r="BZ2" s="88"/>
-      <c r="CA2" s="88"/>
-      <c r="CB2" s="88"/>
-      <c r="CC2" s="88"/>
-      <c r="CD2" s="88"/>
-      <c r="CE2" s="89"/>
+      <c r="BR2" s="95"/>
+      <c r="BS2" s="95"/>
+      <c r="BT2" s="95"/>
+      <c r="BU2" s="95"/>
+      <c r="BV2" s="95"/>
+      <c r="BW2" s="95"/>
+      <c r="BX2" s="95"/>
+      <c r="BY2" s="95"/>
+      <c r="BZ2" s="95"/>
+      <c r="CA2" s="95"/>
+      <c r="CB2" s="95"/>
+      <c r="CC2" s="95"/>
+      <c r="CD2" s="95"/>
+      <c r="CE2" s="96"/>
     </row>
     <row r="3" spans="2:83" ht="18" customHeight="1">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="94" t="s">
+      <c r="F3" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="94" t="s">
+      <c r="G3" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="100" t="s">
+      <c r="I3" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101" t="s">
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="101" t="s">
+      <c r="O3" s="121"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" s="121"/>
+      <c r="S3" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="101"/>
-      <c r="U3" s="101"/>
-      <c r="V3" s="101"/>
-      <c r="W3" s="102"/>
-      <c r="X3" s="103" t="s">
+      <c r="T3" s="121"/>
+      <c r="U3" s="121"/>
+      <c r="V3" s="121"/>
+      <c r="W3" s="122"/>
+      <c r="X3" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="104"/>
-      <c r="AA3" s="104"/>
-      <c r="AB3" s="104"/>
-      <c r="AC3" s="104" t="s">
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="104"/>
-      <c r="AE3" s="104"/>
-      <c r="AF3" s="104"/>
-      <c r="AG3" s="104"/>
-      <c r="AH3" s="104" t="s">
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="104"/>
-      <c r="AJ3" s="104"/>
-      <c r="AK3" s="104"/>
-      <c r="AL3" s="105"/>
-      <c r="AM3" s="106" t="s">
+      <c r="AI3" s="98"/>
+      <c r="AJ3" s="98"/>
+      <c r="AK3" s="98"/>
+      <c r="AL3" s="99"/>
+      <c r="AM3" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="107"/>
-      <c r="AO3" s="107"/>
-      <c r="AP3" s="107"/>
-      <c r="AQ3" s="107"/>
-      <c r="AR3" s="107" t="s">
+      <c r="AN3" s="101"/>
+      <c r="AO3" s="101"/>
+      <c r="AP3" s="101"/>
+      <c r="AQ3" s="101"/>
+      <c r="AR3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="AS3" s="107"/>
-      <c r="AT3" s="107"/>
-      <c r="AU3" s="107"/>
-      <c r="AV3" s="107"/>
-      <c r="AW3" s="107" t="s">
+      <c r="AS3" s="101"/>
+      <c r="AT3" s="101"/>
+      <c r="AU3" s="101"/>
+      <c r="AV3" s="101"/>
+      <c r="AW3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="AX3" s="107"/>
-      <c r="AY3" s="107"/>
-      <c r="AZ3" s="107"/>
-      <c r="BA3" s="108"/>
-      <c r="BB3" s="96" t="s">
+      <c r="AX3" s="101"/>
+      <c r="AY3" s="101"/>
+      <c r="AZ3" s="101"/>
+      <c r="BA3" s="102"/>
+      <c r="BB3" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="BC3" s="97"/>
-      <c r="BD3" s="97"/>
-      <c r="BE3" s="97"/>
-      <c r="BF3" s="97"/>
-      <c r="BG3" s="97" t="s">
+      <c r="BC3" s="92"/>
+      <c r="BD3" s="92"/>
+      <c r="BE3" s="92"/>
+      <c r="BF3" s="92"/>
+      <c r="BG3" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="BH3" s="97"/>
-      <c r="BI3" s="97"/>
-      <c r="BJ3" s="97"/>
-      <c r="BK3" s="97"/>
-      <c r="BL3" s="97" t="s">
+      <c r="BH3" s="92"/>
+      <c r="BI3" s="92"/>
+      <c r="BJ3" s="92"/>
+      <c r="BK3" s="92"/>
+      <c r="BL3" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="97"/>
-      <c r="BN3" s="97"/>
-      <c r="BO3" s="97"/>
-      <c r="BP3" s="109"/>
-      <c r="BQ3" s="96" t="s">
+      <c r="BM3" s="92"/>
+      <c r="BN3" s="92"/>
+      <c r="BO3" s="92"/>
+      <c r="BP3" s="93"/>
+      <c r="BQ3" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="BR3" s="97"/>
-      <c r="BS3" s="97"/>
-      <c r="BT3" s="97"/>
-      <c r="BU3" s="97"/>
-      <c r="BV3" s="97" t="s">
+      <c r="BR3" s="92"/>
+      <c r="BS3" s="92"/>
+      <c r="BT3" s="92"/>
+      <c r="BU3" s="92"/>
+      <c r="BV3" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="BW3" s="97"/>
-      <c r="BX3" s="97"/>
-      <c r="BY3" s="97"/>
-      <c r="BZ3" s="97"/>
-      <c r="CA3" s="97" t="s">
+      <c r="BW3" s="92"/>
+      <c r="BX3" s="92"/>
+      <c r="BY3" s="92"/>
+      <c r="BZ3" s="92"/>
+      <c r="CA3" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="CB3" s="97"/>
-      <c r="CC3" s="97"/>
-      <c r="CD3" s="97"/>
-      <c r="CE3" s="109"/>
+      <c r="CB3" s="92"/>
+      <c r="CC3" s="92"/>
+      <c r="CD3" s="92"/>
+      <c r="CE3" s="93"/>
     </row>
     <row r="4" spans="2:83" ht="18" customHeight="1" thickBot="1">
-      <c r="B4" s="91"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="99"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="119"/>
       <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3210,7 +3219,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="20">
         <f>SUM(H6:H8)/3</f>
-        <v>3.3333333333333333E-2</v>
+        <v>4.3333333333333335E-2</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="22"/>
@@ -3306,7 +3315,7 @@
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="29">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
@@ -3508,7 +3517,7 @@
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="29">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
@@ -3944,7 +3953,7 @@
       <c r="G13" s="41"/>
       <c r="H13" s="42">
         <f>SUM(H14:H17)/4</f>
-        <v>0.26250000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="22"/>
@@ -4040,7 +4049,7 @@
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="29">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
@@ -5458,17 +5467,6 @@
     <row r="33" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BG3:BK3"/>
-    <mergeCell ref="BL3:BP3"/>
-    <mergeCell ref="BQ2:CE2"/>
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BV3:BZ3"/>
-    <mergeCell ref="CA3:CE3"/>
-    <mergeCell ref="AC3:AG3"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AM3:AQ3"/>
-    <mergeCell ref="AR3:AV3"/>
-    <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="X2:AL2"/>
     <mergeCell ref="AM2:BA2"/>
@@ -5485,6 +5483,17 @@
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="S3:W3"/>
     <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AM3:AQ3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="BL3:BP3"/>
+    <mergeCell ref="BQ2:CE2"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BV3:BZ3"/>
+    <mergeCell ref="CA3:CE3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H17 H23:H29">
     <cfRule type="dataBar" priority="2">
@@ -5562,320 +5571,324 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="16384" width="11" style="74"/>
+    <col min="1" max="16384" width="11" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="66" customFormat="1" ht="51.75">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:21" s="125" customFormat="1" ht="51.75">
+      <c r="A1" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="K1" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="M1" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="N1" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="65" t="s">
+      <c r="O1" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="124" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="70" customFormat="1">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:21" s="129" customFormat="1">
+      <c r="A2" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="126" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="135" t="s">
+      <c r="H2" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="67">
+      <c r="I2" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="126">
         <f>COUNTIF(D2:Q2,"P")</f>
-        <v>5</v>
-      </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
+        <v>6</v>
+      </c>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="130" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="136" t="s">
+      <c r="H3" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="71">
+      <c r="I3" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="130">
         <f t="shared" ref="R3:R9" si="0">COUNTIF(D3:Q3,"U")</f>
         <v>0</v>
       </c>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-    </row>
-    <row r="4" spans="1:21" s="70" customFormat="1">
-      <c r="A4" s="67"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="67">
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="U3" s="132"/>
+    </row>
+    <row r="4" spans="1:21" s="129" customFormat="1">
+      <c r="A4" s="126"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="128"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="71"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="71">
+      <c r="A5" s="130"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="131"/>
+      <c r="O5" s="131"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="130">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="70" customFormat="1">
-      <c r="A6" s="67"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="67">
+    <row r="6" spans="1:21" s="129" customFormat="1">
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="71">
+      <c r="A7" s="130"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="131"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="131"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="130">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="70" customFormat="1">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="67">
+    <row r="8" spans="1:21" s="129" customFormat="1">
+      <c r="A8" s="126"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="127"/>
+      <c r="N8" s="127"/>
+      <c r="O8" s="127"/>
+      <c r="P8" s="127"/>
+      <c r="Q8" s="127"/>
+      <c r="R8" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="70" customFormat="1">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
-      <c r="R9" s="71">
+    <row r="9" spans="1:21" s="129" customFormat="1">
+      <c r="A9" s="130"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="131"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
+      <c r="N9" s="131"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="131"/>
+      <c r="Q9" s="131"/>
+      <c r="R9" s="130">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="134" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="134" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="73"/>
-      <c r="B12" s="75" t="s">
+      <c r="A12" s="132"/>
+      <c r="B12" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="134" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="69"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
+      <c r="A13" s="128"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>